<commit_message>
Realice cambios en los beneficiarios en el metodo de importaciones
</commit_message>
<xml_diff>
--- a/Archivos de proyecto/Catalogos pruebas/beneficiarios.xlsx
+++ b/Archivos de proyecto/Catalogos pruebas/beneficiarios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\INSEZAC\Archivos de proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\INSEZAC\Archivos de proyecto\Catalogos pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="109">
   <si>
     <t>CURP</t>
   </si>
@@ -278,15 +278,6 @@
     <t>UAZ, GUADALUPE ,C.P. 98616</t>
   </si>
   <si>
-    <t>AAAE560802MZSLVR07</t>
-  </si>
-  <si>
-    <t>ERNESTINA</t>
-  </si>
-  <si>
-    <t>C DE LA FE</t>
-  </si>
-  <si>
     <t>3200200010000</t>
   </si>
   <si>
@@ -314,9 +305,6 @@
     <t>3200300010000</t>
   </si>
   <si>
-    <t>3200300010001</t>
-  </si>
-  <si>
     <t>320010001</t>
   </si>
   <si>
@@ -342,9 +330,6 @@
   </si>
   <si>
     <t>320010016</t>
-  </si>
-  <si>
-    <t>320010017</t>
   </si>
   <si>
     <t>Email</t>
@@ -785,10 +770,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM12"/>
+  <dimension ref="A1:AM10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
-      <selection activeCell="AM1" sqref="AM1:AM1048576"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AN9" sqref="AN9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -931,22 +916,22 @@
         <v>32</v>
       </c>
       <c r="AH1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AL1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="AI1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="AM1" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:39" ht="24" x14ac:dyDescent="0.25">
@@ -978,10 +963,10 @@
         <v>0</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>38</v>
@@ -1050,13 +1035,15 @@
         <v>2</v>
       </c>
       <c r="AH2" s="8" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="AI2" s="4"/>
       <c r="AJ2" s="4"/>
       <c r="AK2" s="4"/>
       <c r="AL2" s="4"/>
-      <c r="AM2" s="4"/>
+      <c r="AM2" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:39" ht="24" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -1087,10 +1074,10 @@
         <v>0</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>38</v>
@@ -1159,13 +1146,15 @@
         <v>2</v>
       </c>
       <c r="AH3" s="8" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="AI3" s="4"/>
       <c r="AJ3" s="4"/>
       <c r="AK3" s="4"/>
       <c r="AL3" s="4"/>
-      <c r="AM3" s="4"/>
+      <c r="AM3" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:39" ht="24" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -1196,10 +1185,10 @@
         <v>0</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>38</v>
@@ -1268,13 +1257,15 @@
         <v>2</v>
       </c>
       <c r="AH4" s="8" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="AI4" s="4"/>
       <c r="AJ4" s="4"/>
       <c r="AK4" s="4"/>
       <c r="AL4" s="4"/>
-      <c r="AM4" s="4"/>
+      <c r="AM4" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:39" ht="36" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -1305,10 +1296,10 @@
         <v>0</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>38</v>
@@ -1377,13 +1368,15 @@
         <v>2</v>
       </c>
       <c r="AH5" s="8" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="AI5" s="4"/>
       <c r="AJ5" s="4"/>
       <c r="AK5" s="4"/>
       <c r="AL5" s="4"/>
-      <c r="AM5" s="4"/>
+      <c r="AM5" s="4">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:39" ht="36" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -1414,10 +1407,10 @@
         <v>0</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>38</v>
@@ -1486,13 +1479,15 @@
         <v>2</v>
       </c>
       <c r="AH6" s="8" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="AI6" s="4"/>
       <c r="AJ6" s="4"/>
       <c r="AK6" s="4"/>
       <c r="AL6" s="4"/>
-      <c r="AM6" s="4"/>
+      <c r="AM6" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:39" ht="24" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -1523,10 +1518,10 @@
         <v>0</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="L7" s="4" t="s">
         <v>38</v>
@@ -1595,13 +1590,15 @@
         <v>2</v>
       </c>
       <c r="AH7" s="8" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="AI7" s="4"/>
       <c r="AJ7" s="4"/>
       <c r="AK7" s="4"/>
       <c r="AL7" s="4"/>
-      <c r="AM7" s="4"/>
+      <c r="AM7" s="4">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:39" ht="48" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -1632,10 +1629,10 @@
         <v>0</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="L8" s="4" t="s">
         <v>38</v>
@@ -1704,13 +1701,15 @@
         <v>2</v>
       </c>
       <c r="AH8" s="8" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="AI8" s="4"/>
       <c r="AJ8" s="4"/>
       <c r="AK8" s="4"/>
       <c r="AL8" s="4"/>
-      <c r="AM8" s="4"/>
+      <c r="AM8" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="1:39" ht="48" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -1741,10 +1740,10 @@
         <v>0</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>38</v>
@@ -1813,13 +1812,15 @@
         <v>2</v>
       </c>
       <c r="AH9" s="8" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="AI9" s="4"/>
       <c r="AJ9" s="4"/>
       <c r="AK9" s="4"/>
       <c r="AL9" s="4"/>
-      <c r="AM9" s="4"/>
+      <c r="AM9" s="4">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="1:39" ht="24" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -1850,10 +1851,10 @@
         <v>0</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="L10" s="4" t="s">
         <v>38</v>
@@ -1922,284 +1923,20 @@
         <v>2</v>
       </c>
       <c r="AH10" s="8" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="AI10" s="4"/>
       <c r="AJ10" s="4"/>
       <c r="AK10" s="4"/>
       <c r="AL10" s="4"/>
-      <c r="AM10" s="4"/>
-    </row>
-    <row r="11" spans="1:39" ht="24" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E11" s="5">
-        <v>1</v>
-      </c>
-      <c r="F11" s="5">
-        <v>5</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="H11" s="4">
-        <v>14</v>
-      </c>
-      <c r="I11" s="4">
-        <v>0</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="N11" s="4">
-        <v>2</v>
-      </c>
-      <c r="O11" s="4">
-        <v>2</v>
-      </c>
-      <c r="P11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q11" s="4">
-        <v>4</v>
-      </c>
-      <c r="R11" s="4">
-        <v>1</v>
-      </c>
-      <c r="S11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="T11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="U11" s="4">
-        <v>1</v>
-      </c>
-      <c r="V11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="W11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="X11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC11" s="4">
-        <v>2</v>
-      </c>
-      <c r="AD11" s="4">
-        <v>1</v>
-      </c>
-      <c r="AE11" s="4">
-        <v>1</v>
-      </c>
-      <c r="AF11" s="4">
-        <v>1</v>
-      </c>
-      <c r="AG11" s="4">
-        <v>2</v>
-      </c>
-      <c r="AH11" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="AI11" s="4"/>
-      <c r="AJ11" s="4"/>
-      <c r="AK11" s="4"/>
-      <c r="AL11" s="4"/>
-      <c r="AM11" s="4"/>
-    </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12">
-        <f>A12+1</f>
-        <v>2</v>
-      </c>
-      <c r="C12">
-        <f>B12+1</f>
-        <v>3</v>
-      </c>
-      <c r="D12">
-        <f t="shared" ref="D12:AM12" si="0">C12+1</f>
-        <v>4</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="0"/>
+      <c r="AM10" s="4">
         <v>9</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="N12">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="O12">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="P12">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="Q12">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="R12">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="S12">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="T12">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="U12">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="V12">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="W12">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="X12">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="Y12">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="Z12">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="AA12">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="AB12">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="AC12">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="AD12">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="AE12">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="AF12">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="AG12">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="AH12">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="AI12">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="AJ12">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="AK12">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="AL12">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="AM12">
-        <f t="shared" si="0"/>
-        <v>39</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="AH2" r:id="rId1"/>
-    <hyperlink ref="AH3:AH11" r:id="rId2" display="example@hotmail.com"/>
+    <hyperlink ref="AH3:AH10" r:id="rId2" display="example@hotmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
Crud de direcciones completo e importaciones de beneficiarios
</commit_message>
<xml_diff>
--- a/Archivos de proyecto/Catalogos pruebas/beneficiarios.xlsx
+++ b/Archivos de proyecto/Catalogos pruebas/beneficiarios.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="109">
   <si>
     <t>CURP</t>
   </si>
@@ -462,32 +462,36 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
@@ -772,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="AN9" sqref="AN9"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="Z14" sqref="Z14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,6 +798,7 @@
     <col min="15" max="15" width="24.28515625" customWidth="1"/>
     <col min="16" max="16" width="25.5703125" customWidth="1"/>
     <col min="18" max="18" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.85546875" customWidth="1"/>
     <col min="22" max="22" width="17.5703125" customWidth="1"/>
     <col min="23" max="23" width="24.7109375" customWidth="1"/>
     <col min="24" max="24" width="17.7109375" customWidth="1"/>
@@ -816,1120 +821,1174 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AF1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AG1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AH1" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AI1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AK1" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AL1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AM1" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:39" ht="24" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="5">
-        <v>1</v>
-      </c>
-      <c r="F2" s="5">
+      <c r="E2" s="6">
+        <v>1</v>
+      </c>
+      <c r="F2" s="6">
         <v>5</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="5">
         <v>0</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="5">
         <v>0</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="N2" s="4">
-        <v>2</v>
-      </c>
-      <c r="O2" s="4">
-        <v>2</v>
-      </c>
-      <c r="P2" s="4" t="s">
+      <c r="N2" s="5">
+        <v>2</v>
+      </c>
+      <c r="O2" s="5">
+        <v>2</v>
+      </c>
+      <c r="P2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="Q2" s="5">
         <v>4</v>
       </c>
-      <c r="R2" s="4">
-        <v>1</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="U2" s="4">
-        <v>1</v>
-      </c>
-      <c r="V2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="W2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="X2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC2" s="4">
+      <c r="R2" s="5">
+        <v>1</v>
+      </c>
+      <c r="S2" s="5">
+        <v>1</v>
+      </c>
+      <c r="T2" s="5">
+        <v>1</v>
+      </c>
+      <c r="U2" s="5">
+        <v>1</v>
+      </c>
+      <c r="V2" s="5">
+        <v>1</v>
+      </c>
+      <c r="W2" s="5">
+        <v>1</v>
+      </c>
+      <c r="X2" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="5">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="5">
         <v>3</v>
       </c>
-      <c r="AD2" s="4">
-        <v>1</v>
-      </c>
-      <c r="AE2" s="4">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="4">
-        <v>1</v>
-      </c>
-      <c r="AG2" s="4">
+      <c r="AD2" s="5">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="5">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="5">
         <v>2</v>
       </c>
       <c r="AH2" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="AI2" s="4"/>
-      <c r="AJ2" s="4"/>
-      <c r="AK2" s="4"/>
-      <c r="AL2" s="4"/>
-      <c r="AM2" s="4">
+      <c r="AI2" s="9"/>
+      <c r="AJ2" s="5">
+        <v>1</v>
+      </c>
+      <c r="AK2" s="5">
+        <v>2</v>
+      </c>
+      <c r="AL2" s="5">
+        <v>123456789</v>
+      </c>
+      <c r="AM2" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:39" ht="24" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="5">
-        <v>1</v>
-      </c>
-      <c r="F3" s="5">
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+      <c r="F3" s="6">
         <v>5</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="5">
         <v>32</v>
       </c>
-      <c r="I3" s="4">
-        <v>0</v>
-      </c>
-      <c r="J3" s="6" t="s">
+      <c r="I3" s="5">
+        <v>123</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="4">
-        <v>2</v>
-      </c>
-      <c r="O3" s="4">
-        <v>2</v>
-      </c>
-      <c r="P3" s="4" t="s">
+      <c r="N3" s="5">
+        <v>2</v>
+      </c>
+      <c r="O3" s="5">
+        <v>2</v>
+      </c>
+      <c r="P3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="4">
+      <c r="Q3" s="5">
         <v>4</v>
       </c>
-      <c r="R3" s="4">
-        <v>1</v>
-      </c>
-      <c r="S3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="T3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="U3" s="4">
-        <v>1</v>
-      </c>
-      <c r="V3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="W3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="X3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC3" s="4">
-        <v>2</v>
-      </c>
-      <c r="AD3" s="4">
-        <v>1</v>
-      </c>
-      <c r="AE3" s="4">
-        <v>1</v>
-      </c>
-      <c r="AF3" s="4">
-        <v>1</v>
-      </c>
-      <c r="AG3" s="4">
+      <c r="R3" s="5">
+        <v>1</v>
+      </c>
+      <c r="S3" s="5">
+        <v>1</v>
+      </c>
+      <c r="T3" s="5">
+        <v>1</v>
+      </c>
+      <c r="U3" s="5">
+        <v>1</v>
+      </c>
+      <c r="V3" s="5">
+        <v>1</v>
+      </c>
+      <c r="W3" s="5">
+        <v>1</v>
+      </c>
+      <c r="X3" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="5">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="5">
+        <v>2</v>
+      </c>
+      <c r="AD3" s="5">
+        <v>1</v>
+      </c>
+      <c r="AE3" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="5">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="5">
         <v>2</v>
       </c>
       <c r="AH3" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="AI3" s="4"/>
-      <c r="AJ3" s="4"/>
-      <c r="AK3" s="4"/>
-      <c r="AL3" s="4"/>
-      <c r="AM3" s="4">
+      <c r="AI3" s="9"/>
+      <c r="AJ3" s="5">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="5">
+        <v>2</v>
+      </c>
+      <c r="AL3" s="5">
+        <v>123456789</v>
+      </c>
+      <c r="AM3" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:39" ht="24" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="5">
-        <v>1</v>
-      </c>
-      <c r="F4" s="5">
+      <c r="E4" s="6">
+        <v>1</v>
+      </c>
+      <c r="F4" s="6">
         <v>5</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="5">
         <v>149</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="5">
         <v>0</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="N4" s="4">
-        <v>2</v>
-      </c>
-      <c r="O4" s="4">
-        <v>2</v>
-      </c>
-      <c r="P4" s="4" t="s">
+      <c r="N4" s="5">
+        <v>2</v>
+      </c>
+      <c r="O4" s="5">
+        <v>2</v>
+      </c>
+      <c r="P4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="Q4" s="4">
+      <c r="Q4" s="5">
         <v>4</v>
       </c>
-      <c r="R4" s="4">
-        <v>1</v>
-      </c>
-      <c r="S4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="T4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="U4" s="4">
-        <v>1</v>
-      </c>
-      <c r="V4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="W4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="X4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC4" s="4">
+      <c r="R4" s="5">
+        <v>1</v>
+      </c>
+      <c r="S4" s="5">
+        <v>1</v>
+      </c>
+      <c r="T4" s="5">
+        <v>1</v>
+      </c>
+      <c r="U4" s="5">
+        <v>1</v>
+      </c>
+      <c r="V4" s="5">
+        <v>1</v>
+      </c>
+      <c r="W4" s="5">
+        <v>1</v>
+      </c>
+      <c r="X4" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="5">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="5">
         <v>3</v>
       </c>
-      <c r="AD4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AE4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AF4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AG4" s="4">
+      <c r="AD4" s="5">
+        <v>1</v>
+      </c>
+      <c r="AE4" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF4" s="5">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="5">
         <v>2</v>
       </c>
       <c r="AH4" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="AI4" s="4"/>
-      <c r="AJ4" s="4"/>
-      <c r="AK4" s="4"/>
-      <c r="AL4" s="4"/>
-      <c r="AM4" s="4">
+      <c r="AI4" s="9"/>
+      <c r="AJ4" s="5">
+        <v>1</v>
+      </c>
+      <c r="AK4" s="5">
+        <v>2</v>
+      </c>
+      <c r="AL4" s="5">
+        <v>123456789</v>
+      </c>
+      <c r="AM4" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:39" ht="36" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="5">
-        <v>1</v>
-      </c>
-      <c r="F5" s="5">
+      <c r="E5" s="6">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6">
         <v>5</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="5">
         <v>0</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="N5" s="4">
-        <v>2</v>
-      </c>
-      <c r="O5" s="4">
-        <v>1</v>
-      </c>
-      <c r="P5" s="4" t="s">
+      <c r="N5" s="5">
+        <v>2</v>
+      </c>
+      <c r="O5" s="5">
+        <v>1</v>
+      </c>
+      <c r="P5" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="Q5" s="5">
         <v>4</v>
       </c>
-      <c r="R5" s="4">
-        <v>1</v>
-      </c>
-      <c r="S5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="T5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="U5" s="4">
-        <v>1</v>
-      </c>
-      <c r="V5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="W5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="X5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC5" s="4">
+      <c r="R5" s="5">
+        <v>1</v>
+      </c>
+      <c r="S5" s="5">
+        <v>1</v>
+      </c>
+      <c r="T5" s="5">
+        <v>1</v>
+      </c>
+      <c r="U5" s="5">
+        <v>1</v>
+      </c>
+      <c r="V5" s="5">
+        <v>1</v>
+      </c>
+      <c r="W5" s="5">
+        <v>1</v>
+      </c>
+      <c r="X5" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="5">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="5">
         <v>4</v>
       </c>
-      <c r="AD5" s="4">
-        <v>1</v>
-      </c>
-      <c r="AE5" s="4">
-        <v>1</v>
-      </c>
-      <c r="AF5" s="4">
-        <v>1</v>
-      </c>
-      <c r="AG5" s="4">
+      <c r="AD5" s="5">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF5" s="5">
+        <v>1</v>
+      </c>
+      <c r="AG5" s="5">
         <v>2</v>
       </c>
       <c r="AH5" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="AI5" s="4"/>
-      <c r="AJ5" s="4"/>
-      <c r="AK5" s="4"/>
-      <c r="AL5" s="4"/>
-      <c r="AM5" s="4">
+      <c r="AI5" s="9"/>
+      <c r="AJ5" s="5">
+        <v>1</v>
+      </c>
+      <c r="AK5" s="5">
+        <v>2</v>
+      </c>
+      <c r="AL5" s="5">
+        <v>123456789</v>
+      </c>
+      <c r="AM5" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:39" ht="36" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="5">
-        <v>1</v>
-      </c>
-      <c r="F6" s="5">
+      <c r="E6" s="6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="6">
         <v>5</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="5">
         <v>6</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="5">
         <v>0</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="J6" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="K6" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="L6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="M6" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="N6" s="4">
-        <v>2</v>
-      </c>
-      <c r="O6" s="4">
-        <v>1</v>
-      </c>
-      <c r="P6" s="4" t="s">
+      <c r="N6" s="5">
+        <v>2</v>
+      </c>
+      <c r="O6" s="5">
+        <v>1</v>
+      </c>
+      <c r="P6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="Q6" s="4">
+      <c r="Q6" s="5">
         <v>4</v>
       </c>
-      <c r="R6" s="4">
-        <v>1</v>
-      </c>
-      <c r="S6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="T6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="U6" s="4">
-        <v>1</v>
-      </c>
-      <c r="V6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="W6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="X6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC6" s="4">
+      <c r="R6" s="5">
+        <v>1</v>
+      </c>
+      <c r="S6" s="5">
+        <v>1</v>
+      </c>
+      <c r="T6" s="5">
+        <v>1</v>
+      </c>
+      <c r="U6" s="5">
+        <v>1</v>
+      </c>
+      <c r="V6" s="5">
+        <v>1</v>
+      </c>
+      <c r="W6" s="5">
+        <v>1</v>
+      </c>
+      <c r="X6" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="5">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="5">
         <v>3</v>
       </c>
-      <c r="AD6" s="4">
-        <v>1</v>
-      </c>
-      <c r="AE6" s="4">
-        <v>1</v>
-      </c>
-      <c r="AF6" s="4">
-        <v>1</v>
-      </c>
-      <c r="AG6" s="4">
+      <c r="AD6" s="5">
+        <v>1</v>
+      </c>
+      <c r="AE6" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF6" s="5">
+        <v>1</v>
+      </c>
+      <c r="AG6" s="5">
         <v>2</v>
       </c>
       <c r="AH6" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="AI6" s="4"/>
-      <c r="AJ6" s="4"/>
-      <c r="AK6" s="4"/>
-      <c r="AL6" s="4"/>
-      <c r="AM6" s="4">
+      <c r="AI6" s="9"/>
+      <c r="AJ6" s="5">
+        <v>1</v>
+      </c>
+      <c r="AK6" s="5">
+        <v>2</v>
+      </c>
+      <c r="AL6" s="5">
+        <v>123456789</v>
+      </c>
+      <c r="AM6" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:39" ht="24" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="5">
-        <v>1</v>
-      </c>
-      <c r="F7" s="5">
+      <c r="E7" s="6">
+        <v>1</v>
+      </c>
+      <c r="F7" s="6">
         <v>5</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="5">
         <v>6</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="5">
         <v>0</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="K7" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="L7" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="M7" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="N7" s="4">
-        <v>2</v>
-      </c>
-      <c r="O7" s="4">
-        <v>2</v>
-      </c>
-      <c r="P7" s="4" t="s">
+      <c r="N7" s="5">
+        <v>2</v>
+      </c>
+      <c r="O7" s="5">
+        <v>2</v>
+      </c>
+      <c r="P7" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="Q7" s="4">
+      <c r="Q7" s="5">
         <v>4</v>
       </c>
-      <c r="R7" s="4">
-        <v>1</v>
-      </c>
-      <c r="S7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="T7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="U7" s="4">
-        <v>1</v>
-      </c>
-      <c r="V7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="W7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="X7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC7" s="4">
-        <v>2</v>
-      </c>
-      <c r="AD7" s="4">
-        <v>1</v>
-      </c>
-      <c r="AE7" s="4">
-        <v>1</v>
-      </c>
-      <c r="AF7" s="4">
-        <v>1</v>
-      </c>
-      <c r="AG7" s="4">
+      <c r="R7" s="5">
+        <v>1</v>
+      </c>
+      <c r="S7" s="5">
+        <v>1</v>
+      </c>
+      <c r="T7" s="5">
+        <v>1</v>
+      </c>
+      <c r="U7" s="5">
+        <v>1</v>
+      </c>
+      <c r="V7" s="5">
+        <v>1</v>
+      </c>
+      <c r="W7" s="5">
+        <v>1</v>
+      </c>
+      <c r="X7" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="5">
+        <v>1</v>
+      </c>
+      <c r="AC7" s="5">
+        <v>2</v>
+      </c>
+      <c r="AD7" s="5">
+        <v>1</v>
+      </c>
+      <c r="AE7" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF7" s="5">
+        <v>1</v>
+      </c>
+      <c r="AG7" s="5">
         <v>2</v>
       </c>
       <c r="AH7" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="AI7" s="4"/>
-      <c r="AJ7" s="4"/>
-      <c r="AK7" s="4"/>
-      <c r="AL7" s="4"/>
-      <c r="AM7" s="4">
+      <c r="AI7" s="9"/>
+      <c r="AJ7" s="5">
+        <v>1</v>
+      </c>
+      <c r="AK7" s="5">
+        <v>2</v>
+      </c>
+      <c r="AL7" s="5">
+        <v>123456789</v>
+      </c>
+      <c r="AM7" s="5">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:39" ht="48" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="5">
-        <v>1</v>
-      </c>
-      <c r="F8" s="5">
+      <c r="E8" s="6">
+        <v>1</v>
+      </c>
+      <c r="F8" s="6">
         <v>5</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="5">
         <v>475</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="5">
         <v>0</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="K8" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="L8" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="M8" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="N8" s="4">
-        <v>2</v>
-      </c>
-      <c r="O8" s="4">
-        <v>2</v>
-      </c>
-      <c r="P8" s="4" t="s">
+      <c r="N8" s="5">
+        <v>2</v>
+      </c>
+      <c r="O8" s="5">
+        <v>2</v>
+      </c>
+      <c r="P8" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="Q8" s="4">
+      <c r="Q8" s="5">
         <v>4</v>
       </c>
-      <c r="R8" s="4">
-        <v>1</v>
-      </c>
-      <c r="S8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="T8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="U8" s="4">
-        <v>1</v>
-      </c>
-      <c r="V8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="W8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="X8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC8" s="4">
-        <v>2</v>
-      </c>
-      <c r="AD8" s="4">
-        <v>1</v>
-      </c>
-      <c r="AE8" s="4">
-        <v>1</v>
-      </c>
-      <c r="AF8" s="4">
-        <v>1</v>
-      </c>
-      <c r="AG8" s="4">
+      <c r="R8" s="5">
+        <v>1</v>
+      </c>
+      <c r="S8" s="5">
+        <v>1</v>
+      </c>
+      <c r="T8" s="5">
+        <v>1</v>
+      </c>
+      <c r="U8" s="5">
+        <v>1</v>
+      </c>
+      <c r="V8" s="5">
+        <v>1</v>
+      </c>
+      <c r="W8" s="5">
+        <v>1</v>
+      </c>
+      <c r="X8" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="5">
+        <v>1</v>
+      </c>
+      <c r="AC8" s="5">
+        <v>2</v>
+      </c>
+      <c r="AD8" s="5">
+        <v>1</v>
+      </c>
+      <c r="AE8" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF8" s="5">
+        <v>1</v>
+      </c>
+      <c r="AG8" s="5">
         <v>2</v>
       </c>
       <c r="AH8" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="AI8" s="4"/>
-      <c r="AJ8" s="4"/>
-      <c r="AK8" s="4"/>
-      <c r="AL8" s="4"/>
-      <c r="AM8" s="4">
+      <c r="AI8" s="9"/>
+      <c r="AJ8" s="5">
+        <v>1</v>
+      </c>
+      <c r="AK8" s="5">
+        <v>2</v>
+      </c>
+      <c r="AL8" s="5">
+        <v>123456789</v>
+      </c>
+      <c r="AM8" s="5">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:39" ht="48" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E9" s="5">
-        <v>1</v>
-      </c>
-      <c r="F9" s="5">
+      <c r="E9" s="6">
+        <v>1</v>
+      </c>
+      <c r="F9" s="6">
         <v>5</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="5">
         <v>7</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="5">
         <v>0</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="J9" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="K9" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="L9" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="M9" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="N9" s="4">
-        <v>2</v>
-      </c>
-      <c r="O9" s="4">
-        <v>2</v>
-      </c>
-      <c r="P9" s="4" t="s">
+      <c r="N9" s="5">
+        <v>2</v>
+      </c>
+      <c r="O9" s="5">
+        <v>2</v>
+      </c>
+      <c r="P9" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="Q9" s="4">
+      <c r="Q9" s="5">
         <v>4</v>
       </c>
-      <c r="R9" s="4">
-        <v>1</v>
-      </c>
-      <c r="S9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="T9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="U9" s="4">
-        <v>1</v>
-      </c>
-      <c r="V9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="W9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="X9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC9" s="4">
+      <c r="R9" s="5">
+        <v>1</v>
+      </c>
+      <c r="S9" s="5">
+        <v>1</v>
+      </c>
+      <c r="T9" s="5">
+        <v>1</v>
+      </c>
+      <c r="U9" s="5">
+        <v>1</v>
+      </c>
+      <c r="V9" s="5">
+        <v>1</v>
+      </c>
+      <c r="W9" s="5">
+        <v>1</v>
+      </c>
+      <c r="X9" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB9" s="5">
+        <v>1</v>
+      </c>
+      <c r="AC9" s="5">
         <v>4</v>
       </c>
-      <c r="AD9" s="4">
-        <v>1</v>
-      </c>
-      <c r="AE9" s="4">
-        <v>1</v>
-      </c>
-      <c r="AF9" s="4">
-        <v>1</v>
-      </c>
-      <c r="AG9" s="4">
+      <c r="AD9" s="5">
+        <v>1</v>
+      </c>
+      <c r="AE9" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF9" s="5">
+        <v>1</v>
+      </c>
+      <c r="AG9" s="5">
         <v>2</v>
       </c>
       <c r="AH9" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="AI9" s="4"/>
-      <c r="AJ9" s="4"/>
-      <c r="AK9" s="4"/>
-      <c r="AL9" s="4"/>
-      <c r="AM9" s="4">
+      <c r="AI9" s="9"/>
+      <c r="AJ9" s="5">
+        <v>1</v>
+      </c>
+      <c r="AK9" s="5">
+        <v>2</v>
+      </c>
+      <c r="AL9" s="5">
+        <v>123456789</v>
+      </c>
+      <c r="AM9" s="5">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:39" ht="24" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E10" s="5">
-        <v>1</v>
-      </c>
-      <c r="F10" s="5">
+      <c r="E10" s="6">
+        <v>1</v>
+      </c>
+      <c r="F10" s="6">
         <v>5</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="5">
         <v>7</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="5">
         <v>0</v>
       </c>
-      <c r="J10" s="6" t="s">
+      <c r="J10" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="K10" s="7" t="s">
+      <c r="K10" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="L10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="M10" s="4" t="s">
+      <c r="M10" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="N10" s="4">
-        <v>2</v>
-      </c>
-      <c r="O10" s="4">
-        <v>1</v>
-      </c>
-      <c r="P10" s="4" t="s">
+      <c r="N10" s="5">
+        <v>2</v>
+      </c>
+      <c r="O10" s="5">
+        <v>1</v>
+      </c>
+      <c r="P10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="Q10" s="4">
+      <c r="Q10" s="5">
         <v>4</v>
       </c>
-      <c r="R10" s="4">
-        <v>1</v>
-      </c>
-      <c r="S10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="T10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="U10" s="4">
-        <v>1</v>
-      </c>
-      <c r="V10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="W10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="X10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC10" s="4">
+      <c r="R10" s="5">
+        <v>1</v>
+      </c>
+      <c r="S10" s="5">
+        <v>1</v>
+      </c>
+      <c r="T10" s="5">
+        <v>1</v>
+      </c>
+      <c r="U10" s="5">
+        <v>1</v>
+      </c>
+      <c r="V10" s="5">
+        <v>1</v>
+      </c>
+      <c r="W10" s="5">
+        <v>1</v>
+      </c>
+      <c r="X10" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z10" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB10" s="5">
+        <v>1</v>
+      </c>
+      <c r="AC10" s="5">
         <v>4</v>
       </c>
-      <c r="AD10" s="4">
-        <v>1</v>
-      </c>
-      <c r="AE10" s="4">
-        <v>1</v>
-      </c>
-      <c r="AF10" s="4">
-        <v>1</v>
-      </c>
-      <c r="AG10" s="4">
+      <c r="AD10" s="5">
+        <v>1</v>
+      </c>
+      <c r="AE10" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF10" s="5">
+        <v>1</v>
+      </c>
+      <c r="AG10" s="5">
         <v>2</v>
       </c>
       <c r="AH10" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="AI10" s="4"/>
-      <c r="AJ10" s="4"/>
-      <c r="AK10" s="4"/>
-      <c r="AL10" s="4"/>
-      <c r="AM10" s="4">
+      <c r="AI10" s="9"/>
+      <c r="AJ10" s="5">
+        <v>1</v>
+      </c>
+      <c r="AK10" s="5">
+        <v>2</v>
+      </c>
+      <c r="AL10" s="5">
+        <v>123456789</v>
+      </c>
+      <c r="AM10" s="5">
         <v>9</v>
       </c>
     </row>

</xml_diff>